<commit_message>
přepracovaná verze, rozdělení na funkce
</commit_message>
<xml_diff>
--- a/databaze_filmu.xlsx
+++ b/databaze_filmu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3c678b8341a1804/Dokumenty/carousely/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="13_ncr:1_{F0DD17AA-57C3-401E-A619-37D4E16B6A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71575A5C-A712-44AE-9749-E28D505B270C}"/>
+  <xr:revisionPtr revIDLastSave="240" documentId="13_ncr:1_{F0DD17AA-57C3-401E-A619-37D4E16B6A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A5C0E0F-EC59-45AA-96C0-5548B97AEAE3}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="databaze_filmu" sheetId="3" r:id="rId1"/>
@@ -1476,7 +1476,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="VŠECHNY_FILMY" displayName="VŠECHNY_FILMY" ref="A1:T170">
-  <autoFilter ref="A1:T170" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}"/>
+  <autoFilter ref="A1:T170" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T170">
     <sortCondition ref="A1:A170"/>
   </sortState>
@@ -1711,9 +1717,9 @@
   </sheetPr>
   <dimension ref="A1:T197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U163" sqref="U163"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1802,10 +1808,10 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <f t="shared" ref="A2:A33" ca="1" si="0">RAND()</f>
-        <v>0.92235655832425711</v>
+        <v>0.56131895000087428</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>57</v>
@@ -1865,10 +1871,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9227435974657644</v>
+        <v>0.11884082732671319</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>29</v>
@@ -1928,10 +1934,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9299054860233148</v>
+        <v>0.3201540440127042</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
@@ -1991,10 +1997,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99333240485764707</v>
+        <v>0.30019024750288592</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>54</v>
@@ -2054,16 +2060,16 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.36437187084221967</v>
+        <v>0.72668298833018763</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>153</v>
@@ -2117,10 +2123,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64879541012090758</v>
+        <v>0.80307263875865631</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>98</v>
@@ -2180,10 +2186,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81370753745171565</v>
+        <v>0.63531883990805471</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>104</v>
@@ -2243,10 +2249,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24035472003423641</v>
+        <v>0.40200148366477106</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>48</v>
@@ -2306,10 +2312,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81757245305100634</v>
+        <v>0.40409063664739286</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>147</v>
@@ -2369,10 +2375,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.58807364307867416</v>
+        <v>0.20313217245604376</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>150</v>
@@ -2432,10 +2438,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94616726016072061</v>
+        <v>0.11076356144614485</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>145</v>
@@ -2495,10 +2501,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3383439727505162E-2</v>
+        <v>0.57162049056511122</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>123</v>
@@ -2558,10 +2564,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11005499032683674</v>
+        <v>0.31124754773189844</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>168</v>
@@ -2624,7 +2630,7 @@
     <row r="15" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25281358944039134</v>
+        <v>0.29013224642469571</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -2684,10 +2690,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37234659750021648</v>
+        <v>0.15513632680714473</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>116</v>
@@ -2747,10 +2753,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72392292294294858</v>
+        <v>0.45792037956528142</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>143</v>
@@ -2810,10 +2816,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70953353595548219</v>
+        <v>0.75022088293955147</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>152</v>
@@ -2873,10 +2879,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75251966819156491</v>
+        <v>0.93766660618215969</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>7</v>
@@ -2936,10 +2942,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30452576757986782</v>
+        <v>0.69791234370536259</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>115</v>
@@ -2999,10 +3005,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70093701443196221</v>
+        <v>0.4213226437789771</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>141</v>
@@ -3062,10 +3068,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7656477535525078</v>
+        <v>0.44673155895267869</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>62</v>
@@ -3125,10 +3131,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56561903667945235</v>
+        <v>0.61300993286841476</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>87</v>
@@ -3188,10 +3194,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14870852215118913</v>
+        <v>0.74994037173939465</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>89</v>
@@ -3251,10 +3257,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85339512233228454</v>
+        <v>0.45244932307441965</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>132</v>
@@ -3314,10 +3320,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85276420969000355</v>
+        <v>0.20586130570088412</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>10</v>
@@ -3377,10 +3383,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7619376760753156</v>
+        <v>0.54203309719093506</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>109</v>
@@ -3440,10 +3446,10 @@
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89513142451297512</v>
+        <v>0.54494816369420562</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>172</v>
@@ -3503,10 +3509,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85851522570261796</v>
+        <v>0.66336728066567052</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>91</v>
@@ -3566,16 +3572,16 @@
         <v>153</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75387595863603207</v>
+        <v>0.84948352571860852</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>170</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>153</v>
@@ -3629,10 +3635,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15922854099300554</v>
+        <v>5.607640585618523E-2</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>21</v>
@@ -3692,10 +3698,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3085703285707702E-2</v>
+        <v>0.23645058889101456</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>9</v>
@@ -3755,10 +3761,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6087757579288771E-2</v>
+        <v>0.42810925047961856</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>53</v>
@@ -3818,10 +3824,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <f t="shared" ref="A34:A65" ca="1" si="1">RAND()</f>
-        <v>0.63920534430255382</v>
+        <v>0.6927176034640542</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>122</v>
@@ -3881,10 +3887,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21449741664811095</v>
+        <v>0.81955851801447155</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>45</v>
@@ -3944,10 +3950,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16359987431846834</v>
+        <v>0.66491315760834213</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>130</v>
@@ -4007,10 +4013,10 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52451521889253783</v>
+        <v>0.35576246987923843</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>110</v>
@@ -4070,10 +4076,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12701628509396945</v>
+        <v>0.20570458541962355</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>127</v>
@@ -4133,10 +4139,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.14784978878638877</v>
+        <v>0.72794033314332862</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>31</v>
@@ -4196,10 +4202,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2801480725782014</v>
+        <v>0.22872710779440897</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>159</v>
@@ -4262,7 +4268,7 @@
     <row r="41" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20224031666133024</v>
+        <v>0.76074872558348805</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>96</v>
@@ -4322,10 +4328,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76580999084570889</v>
+        <v>0.73801180099067276</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>19</v>
@@ -4385,10 +4391,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5912969639995795E-2</v>
+        <v>0.11001566746635871</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>163</v>
@@ -4448,10 +4454,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72599207808735711</v>
+        <v>0.48247319260892163</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>13</v>
@@ -4511,10 +4517,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85686900219594886</v>
+        <v>0.65856550650463996</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>44</v>
@@ -4574,10 +4580,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22016923731468319</v>
+        <v>0.88869370633392863</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>41</v>
@@ -4637,10 +4643,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26003328874365428</v>
+        <v>0.57460087699263418</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>28</v>
@@ -4700,16 +4706,16 @@
         <v>153</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42000897617976796</v>
+        <v>0.41289335517690184</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>153</v>
@@ -4763,10 +4769,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85071179639371952</v>
+        <v>0.40041547831764268</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>95</v>
@@ -4826,10 +4832,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58530238820658487</v>
+        <v>0.75487847181288914</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>47</v>
@@ -4889,10 +4895,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49524340949193935</v>
+        <v>0.55947166534618165</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>58</v>
@@ -4952,10 +4958,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31924803409712244</v>
+        <v>0.449603167417848</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>40</v>
@@ -5015,10 +5021,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34463317461237719</v>
+        <v>0.35330499152905559</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>99</v>
@@ -5078,10 +5084,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84414641507726162</v>
+        <v>0.93541450953564664</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>111</v>
@@ -5141,10 +5147,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71515328192945982</v>
+        <v>0.71609359955229357</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>135</v>
@@ -5204,10 +5210,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85722318539134212</v>
+        <v>0.84760480636344082</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>25</v>
@@ -5267,10 +5273,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.51381515191952642</v>
+        <v>0.65367102306826597</v>
       </c>
       <c r="B57" s="21" t="s">
         <v>171</v>
@@ -5330,10 +5336,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88090519794850963</v>
+        <v>0.32290482548577415</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>43</v>
@@ -5393,10 +5399,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38483065730954691</v>
+        <v>1.3809031256545978E-2</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>139</v>
@@ -5456,10 +5462,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10837946901753437</v>
+        <v>0.26560503669417868</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>26</v>
@@ -5522,7 +5528,7 @@
     <row r="61" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58479748154158473</v>
+        <v>0.72146300890191017</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>37</v>
@@ -5585,7 +5591,7 @@
     <row r="62" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25153792226694183</v>
+        <v>0.947982759193435</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>121</v>
@@ -5645,10 +5651,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>6.777822154651969E-2</v>
+        <v>0.82645520248558646</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>137</v>
@@ -5708,10 +5714,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3831507469331048E-2</v>
+        <v>0.99287772639623761</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>126</v>
@@ -5771,10 +5777,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38325415788948536</v>
+        <v>0.76890431602130849</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>30</v>
@@ -5834,10 +5840,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <f t="shared" ref="A66:A97" ca="1" si="2">RAND()</f>
-        <v>0.69230280842726</v>
+        <v>0.85094907142466469</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>136</v>
@@ -5897,10 +5903,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26168031148652304</v>
+        <v>0.96900081382839998</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>138</v>
@@ -5960,10 +5966,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.69638652579825655</v>
+        <v>0.7995594114088016</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>113</v>
@@ -6023,10 +6029,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.19853421867874799</v>
+        <v>0.63837492907680526</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>85</v>
@@ -6086,10 +6092,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.68966083772576769</v>
+        <v>0.24551320082324934</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>79</v>
@@ -6149,10 +6155,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26376814007349225</v>
+        <v>3.676946309415452E-2</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>15</v>
@@ -6212,10 +6218,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1053685529609503E-2</v>
+        <v>0.7189206715490678</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>59</v>
@@ -6275,10 +6281,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.15522255946789654</v>
+        <v>0.51202391628683208</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>156</v>
@@ -6338,10 +6344,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.44698331427050653</v>
+        <v>0.42142736139162851</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>129</v>
@@ -6401,10 +6407,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.22623837254471191</v>
+        <v>0.51410777687375753</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>148</v>
@@ -6464,10 +6470,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>2.7323745335758876E-3</v>
+        <v>0.95396061405432953</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>169</v>
@@ -6527,10 +6533,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.93582508891010074</v>
+        <v>0.39420354444262495</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>94</v>
@@ -6590,10 +6596,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.95422185246867963</v>
+        <v>0.28693120359343305</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>101</v>
@@ -6653,10 +6659,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.23190633139439198</v>
+        <v>0.2285343209817069</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>162</v>
@@ -6716,10 +6722,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.17112409186351651</v>
+        <v>0.6857196534745128</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>50</v>
@@ -6779,10 +6785,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.87235600964313642</v>
+        <v>0.90510551160236818</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>165</v>
@@ -6842,10 +6848,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.42688729934260417</v>
+        <v>8.1074100168581742E-2</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>175</v>
@@ -6905,10 +6911,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.5299627816655138</v>
+        <v>0.78396219982386905</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>161</v>
@@ -6968,10 +6974,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.23645946988276756</v>
+        <v>0.89379098202099228</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>119</v>
@@ -7031,10 +7037,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.99469298602496037</v>
+        <v>9.9540835564603136E-2</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>23</v>
@@ -7094,10 +7100,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.12965091233154125</v>
+        <v>0.61463577313106899</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>117</v>
@@ -7157,10 +7163,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85799739088012716</v>
+        <v>0.14125290843094351</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>17</v>
@@ -7223,7 +7229,7 @@
     <row r="88" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.68058732655734644</v>
+        <v>0.7571194770741132</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>178</v>
@@ -7283,10 +7289,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.78484121679256325</v>
+        <v>4.8092709127000366E-2</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>134</v>
@@ -7346,10 +7352,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.8499858104381055</v>
+        <v>0.53165020165687638</v>
       </c>
       <c r="B90" s="21" t="s">
         <v>173</v>
@@ -7409,10 +7415,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.91471761223695314</v>
+        <v>0.89825869096537592</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>118</v>
@@ -7472,10 +7478,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.13369688203503372</v>
+        <v>0.49931715874760618</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>103</v>
@@ -7535,10 +7541,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.64068653523807895</v>
+        <v>0.63082951396802611</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>34</v>
@@ -7598,10 +7604,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.35789460203206247</v>
+        <v>0.34436631389024919</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>125</v>
@@ -7661,10 +7667,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.58860019717707535</v>
+        <v>0.85038672164470364</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>102</v>
@@ -7724,10 +7730,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.3868980734131684</v>
+        <v>0.37866004944059806</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>149</v>
@@ -7787,10 +7793,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.70632333457293783</v>
+        <v>0.86403585354874257</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>38</v>
@@ -7850,10 +7856,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="8">
         <f t="shared" ref="A98:A129" ca="1" si="3">RAND()</f>
-        <v>0.69440040579122608</v>
+        <v>0.43682808527160666</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>55</v>
@@ -7913,10 +7919,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.91556514101691444</v>
+        <v>4.5047510179202166E-2</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>8</v>
@@ -7976,10 +7982,10 @@
         <v>154</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.25825147210125643</v>
+        <v>0.81794159223574092</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>166</v>
@@ -8039,10 +8045,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13523392163890946</v>
+        <v>0.30495880055738178</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>35</v>
@@ -8102,10 +8108,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.48827917988167657</v>
+        <v>0.36721279031637299</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>11</v>
@@ -8165,10 +8171,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.43645167039444321</v>
+        <v>0.43335581016939351</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>22</v>
@@ -8228,10 +8234,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.37512423672223438</v>
+        <v>0.50566143775732819</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>84</v>
@@ -8291,10 +8297,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.18026007104250497</v>
+        <v>0.99569191221347397</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>77</v>
@@ -8354,10 +8360,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.96899014175903198</v>
+        <v>0.59982864877726727</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>158</v>
@@ -8417,10 +8423,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.27696817170588672</v>
+        <v>0.90048783197926596</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>83</v>
@@ -8480,10 +8486,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.23123972318413744</v>
+        <v>0.2943438162225448</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>51</v>
@@ -8543,10 +8549,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.65805801816956677</v>
+        <v>0.75458037257893684</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>36</v>
@@ -8606,10 +8612,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.57199322883523906</v>
+        <v>0.33825562530743758</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>174</v>
@@ -8669,10 +8675,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.4531334774679342</v>
+        <v>0.93604525121117044</v>
       </c>
       <c r="B111" s="5" t="s">
         <v>49</v>
@@ -8732,10 +8738,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.99476989146840111</v>
+        <v>3.375435807187166E-2</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>120</v>
@@ -8795,10 +8801,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>7.4604675724777691E-2</v>
+        <v>6.781051746453659E-2</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>140</v>
@@ -8858,10 +8864,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.37959102906965836</v>
+        <v>0.10383243153597033</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>142</v>
@@ -8921,10 +8927,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.18278911455675162</v>
+        <v>0.50996415236341386</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>86</v>
@@ -8984,10 +8990,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.29433618761425928</v>
+        <v>0.16214916962433967</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>81</v>
@@ -9047,10 +9053,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.46301845044073786</v>
+        <v>0.73472477852915141</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>157</v>
@@ -9110,10 +9116,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3324218085157047E-2</v>
+        <v>0.74686532103330372</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>80</v>
@@ -9176,7 +9182,7 @@
     <row r="119" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.71869757331858575</v>
+        <v>0.54966684377843711</v>
       </c>
       <c r="B119" s="5" t="s">
         <v>106</v>
@@ -9236,10 +9242,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.99546885221639214</v>
+        <v>0.95205634622667423</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>32</v>
@@ -9299,10 +9305,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>2.1403936133685297E-2</v>
+        <v>0.66590812941555222</v>
       </c>
       <c r="B121" s="5" t="s">
         <v>1</v>
@@ -9362,10 +9368,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.88844427946640236</v>
+        <v>0.45391295552704725</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>92</v>
@@ -9425,10 +9431,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.97562967689344515</v>
+        <v>0.84777467771142134</v>
       </c>
       <c r="B123" s="5" t="s">
         <v>24</v>
@@ -9488,10 +9494,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.24427115328950877</v>
+        <v>0.89734780723948027</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>78</v>
@@ -9554,7 +9560,7 @@
     <row r="125" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.60297625988312586</v>
+        <v>0.58717063355476562</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>133</v>
@@ -9617,7 +9623,7 @@
     <row r="126" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.28103573719390595</v>
+        <v>0.15258015437269346</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>151</v>
@@ -9677,10 +9683,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>0.42421703888074036</v>
+        <v>0.57452449916336445</v>
       </c>
       <c r="B127" s="5" t="s">
         <v>100</v>
@@ -9740,10 +9746,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>4.1071549584025591E-2</v>
+        <v>0.5705723661316594</v>
       </c>
       <c r="B128" s="5" t="s">
         <v>46</v>
@@ -9803,10 +9809,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="8">
         <f t="shared" ca="1" si="3"/>
-        <v>3.2694768006781172E-2</v>
+        <v>0.5398667394047485</v>
       </c>
       <c r="B129" s="5" t="s">
         <v>177</v>
@@ -9866,10 +9872,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="8">
         <f t="shared" ref="A130:A163" ca="1" si="4">RAND()</f>
-        <v>0.10132189859217144</v>
+        <v>0.57420455349983723</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>88</v>
@@ -9929,16 +9935,16 @@
         <v>153</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.87772552787344305</v>
+        <v>0.56313722145167244</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>153</v>
@@ -9992,10 +9998,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.66585493691026765</v>
+        <v>6.1316204577569922E-2</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>155</v>
@@ -10055,10 +10061,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.1987633461257553</v>
+        <v>0.83457736297307317</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>39</v>
@@ -10118,10 +10124,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>1.7297904348708371E-2</v>
+        <v>0.15273790877237492</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>16</v>
@@ -10181,10 +10187,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.2915615943737363</v>
+        <v>0.44130997173697684</v>
       </c>
       <c r="B135" s="5" t="s">
         <v>61</v>
@@ -10244,10 +10250,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.97147222991384108</v>
+        <v>0.26383700577628622</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>108</v>
@@ -10307,10 +10313,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.39046702901187713</v>
+        <v>0.52663047455742384</v>
       </c>
       <c r="B137" s="5" t="s">
         <v>60</v>
@@ -10370,10 +10376,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.67261062270817429</v>
+        <v>0.75477865303817793</v>
       </c>
       <c r="B138" s="5" t="s">
         <v>124</v>
@@ -10433,10 +10439,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>8.4694166969274232E-2</v>
+        <v>0.97204838307179686</v>
       </c>
       <c r="B139" s="5" t="s">
         <v>164</v>
@@ -10496,10 +10502,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.87894358662457006</v>
+        <v>6.791335308520341E-2</v>
       </c>
       <c r="B140" s="5" t="s">
         <v>105</v>
@@ -10559,10 +10565,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.83814914534581064</v>
+        <v>0.7342040612202172</v>
       </c>
       <c r="B141" s="5" t="s">
         <v>128</v>
@@ -10625,7 +10631,7 @@
     <row r="142" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.37377937230427527</v>
+        <v>7.7307422430512696E-2</v>
       </c>
       <c r="B142" s="5" t="s">
         <v>176</v>
@@ -10685,10 +10691,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.5600109437791424</v>
+        <v>0.61117532867474367</v>
       </c>
       <c r="B143" s="5" t="s">
         <v>56</v>
@@ -10748,10 +10754,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.70219103798742666</v>
+        <v>0.8614083110047891</v>
       </c>
       <c r="B144" s="5" t="s">
         <v>144</v>
@@ -10811,10 +10817,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.75050169478692996</v>
+        <v>6.6279104673826472E-2</v>
       </c>
       <c r="B145" s="5" t="s">
         <v>167</v>
@@ -10874,10 +10880,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.16149816099562864</v>
+        <v>0.12930571351915998</v>
       </c>
       <c r="B146" s="5" t="s">
         <v>93</v>
@@ -10937,10 +10943,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.12076896470788256</v>
+        <v>0.35249475747024628</v>
       </c>
       <c r="B147" s="5" t="s">
         <v>4</v>
@@ -11000,10 +11006,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.54695152001597525</v>
+        <v>0.94528202823968588</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>52</v>
@@ -11063,10 +11069,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>5.7251146513799034E-2</v>
+        <v>3.6615099738946943E-3</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>18</v>
@@ -11126,10 +11132,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.78659219229581612</v>
+        <v>7.7071523648872708E-2</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>33</v>
@@ -11189,10 +11195,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.59546312556670111</v>
+        <v>0.13037286265455705</v>
       </c>
       <c r="B151" s="5" t="s">
         <v>0</v>
@@ -11252,10 +11258,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.16988236598494244</v>
+        <v>0.5139694349959314</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>97</v>
@@ -11315,10 +11321,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.4532680607094538</v>
+        <v>0.94173661870212222</v>
       </c>
       <c r="B153" s="5" t="s">
         <v>42</v>
@@ -11378,10 +11384,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.89320965551139309</v>
+        <v>0.24614662446346702</v>
       </c>
       <c r="B154" s="5" t="s">
         <v>146</v>
@@ -11441,10 +11447,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.46532050010079429</v>
+        <v>0.70925963361743982</v>
       </c>
       <c r="B155" s="5" t="s">
         <v>27</v>
@@ -11504,10 +11510,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.23804658434669856</v>
+        <v>0.34812794088505594</v>
       </c>
       <c r="B156" s="7" t="s">
         <v>107</v>
@@ -11567,10 +11573,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.88565344500639065</v>
+        <v>0.87119821456243796</v>
       </c>
       <c r="B157" s="5" t="s">
         <v>82</v>
@@ -11630,10 +11636,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.76043148373130676</v>
+        <v>0.37737696975596779</v>
       </c>
       <c r="B158" s="5" t="s">
         <v>20</v>
@@ -11693,10 +11699,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.97544756143489253</v>
+        <v>0.73273687697316003</v>
       </c>
       <c r="B159" s="5" t="s">
         <v>179</v>
@@ -11756,16 +11762,16 @@
         <v>153</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.59861355146760387</v>
+        <v>0.59442329020288742</v>
       </c>
       <c r="B160" s="5" t="s">
         <v>180</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D160" s="6" t="s">
         <v>153</v>
@@ -11819,10 +11825,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.92070468938486305</v>
+        <v>0.38822066761868679</v>
       </c>
       <c r="B161" s="5" t="s">
         <v>181</v>
@@ -11882,10 +11888,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.17727528006736237</v>
+        <v>0.54630801284317398</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>182</v>
@@ -11945,10 +11951,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.68412127656059829</v>
+        <v>0.61656980355869995</v>
       </c>
       <c r="B163" s="5" t="s">
         <v>183</v>
@@ -12008,7 +12014,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="8"/>
       <c r="B164" s="5"/>
       <c r="C164" s="6" t="s">
@@ -12066,7 +12072,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="8"/>
       <c r="B165" s="5"/>
       <c r="C165" s="6" t="s">
@@ -12124,7 +12130,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="8"/>
       <c r="B166" s="5"/>
       <c r="C166" s="6" t="s">
@@ -12182,7 +12188,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="8"/>
       <c r="B167" s="5"/>
       <c r="C167" s="6" t="s">
@@ -12240,7 +12246,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="8"/>
       <c r="B168" s="5"/>
       <c r="C168" s="6" t="s">
@@ -12298,7 +12304,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="17"/>
       <c r="B169" s="5"/>
       <c r="C169" s="6" t="s">
@@ -12356,7 +12362,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:20" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="20"/>
       <c r="B170" s="19"/>
       <c r="C170" s="6" t="s">

</xml_diff>